<commit_message>
TICC-270 - no CreditNote
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v8.6.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v8.6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\peppol-edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838FF991-532B-4136-9BB7-089AC0129A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CFB1F3-A985-4BD4-B0E5-127015EFB053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24750" yWindow="870" windowWidth="20280" windowHeight="20010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Document Type" sheetId="5" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Document Type'!$A$1:$L$231</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Document Type'!$A$1:$L$229</definedName>
     <definedName name="_ftn1" localSheetId="0">'Document Type'!#REF!</definedName>
     <definedName name="_ftn2" localSheetId="0">'Document Type'!#REF!</definedName>
     <definedName name="_ftn3" localSheetId="0">'Document Type'!#REF!</definedName>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1768" uniqueCount="633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1752" uniqueCount="631">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -1962,12 +1962,6 @@
   </si>
   <si>
     <t>JP PINT Invoice v1.0</t>
-  </si>
-  <si>
-    <t>JP PINT CreditNote v1.0</t>
-  </si>
-  <si>
-    <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:peppol:pint:billing-1@jp-1::2.1</t>
   </si>
   <si>
     <t>JP BIS Invoice for Non-tax Registered Businesses</t>
@@ -2634,11 +2628,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
-  <dimension ref="A1:L231"/>
+  <dimension ref="A1:L229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A213" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J223" sqref="J223"/>
+      <selection pane="bottomLeft" activeCell="A223" sqref="A223:XFD229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -9825,13 +9819,13 @@
     </row>
     <row r="227" spans="1:12">
       <c r="A227" t="s">
-        <v>629</v>
-      </c>
-      <c r="B227" s="4" t="s">
-        <v>56</v>
+        <v>535</v>
+      </c>
+      <c r="B227" s="5" t="s">
+        <v>620</v>
       </c>
       <c r="C227" s="5" t="s">
-        <v>630</v>
+        <v>536</v>
       </c>
       <c r="D227" s="28" t="s">
         <v>601</v>
@@ -9852,15 +9846,15 @@
         <v>117</v>
       </c>
       <c r="L227" s="5" t="s">
-        <v>623</v>
+        <v>539</v>
       </c>
     </row>
     <row r="228" spans="1:12">
       <c r="A228" t="s">
         <v>629</v>
       </c>
-      <c r="B228" s="5" t="s">
-        <v>620</v>
+      <c r="B228" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="C228" s="5" t="s">
         <v>630</v>
@@ -9889,13 +9883,13 @@
     </row>
     <row r="229" spans="1:12">
       <c r="A229" t="s">
-        <v>535</v>
+        <v>629</v>
       </c>
       <c r="B229" s="5" t="s">
         <v>620</v>
       </c>
       <c r="C229" s="5" t="s">
-        <v>536</v>
+        <v>630</v>
       </c>
       <c r="D229" s="28" t="s">
         <v>601</v>
@@ -9916,75 +9910,11 @@
         <v>117</v>
       </c>
       <c r="L229" s="5" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="230" spans="1:12">
-      <c r="A230" t="s">
-        <v>631</v>
-      </c>
-      <c r="B230" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C230" s="5" t="s">
-        <v>632</v>
-      </c>
-      <c r="D230" s="28" t="s">
-        <v>601</v>
-      </c>
-      <c r="E230" s="24" t="s">
-        <v>369</v>
-      </c>
-      <c r="H230" s="5" t="s">
-        <v>622</v>
-      </c>
-      <c r="I230" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J230" s="24">
-        <v>3</v>
-      </c>
-      <c r="K230" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="L230" s="5" t="s">
         <v>623</v>
       </c>
     </row>
-    <row r="231" spans="1:12">
-      <c r="A231" t="s">
-        <v>631</v>
-      </c>
-      <c r="B231" s="5" t="s">
-        <v>620</v>
-      </c>
-      <c r="C231" s="5" t="s">
-        <v>632</v>
-      </c>
-      <c r="D231" s="28" t="s">
-        <v>601</v>
-      </c>
-      <c r="E231" s="24" t="s">
-        <v>369</v>
-      </c>
-      <c r="H231" s="5" t="s">
-        <v>622</v>
-      </c>
-      <c r="I231" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J231" s="24">
-        <v>3</v>
-      </c>
-      <c r="K231" s="24" t="s">
-        <v>117</v>
-      </c>
-      <c r="L231" s="5" t="s">
-        <v>623</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:L231" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L229" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added A-NZ PINT Invoices; TICC-279
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v8.6.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v8.6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\peppol-edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88DEA58-64CF-4991-B4EA-D4A5A71B9995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3298D53-E276-4D38-9C5C-B0570F183ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Document Type" sheetId="5" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Document Type'!$A$1:$L$229</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Document Type'!$A$1:$L$237</definedName>
     <definedName name="_ftn1" localSheetId="0">'Document Type'!#REF!</definedName>
     <definedName name="_ftn2" localSheetId="0">'Document Type'!#REF!</definedName>
     <definedName name="_ftn3" localSheetId="0">'Document Type'!#REF!</definedName>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1752" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1816" uniqueCount="640">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -1968,6 +1968,33 @@
   </si>
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:peppol:pint:nontaxinvoice-1@jp-1::2.1</t>
+  </si>
+  <si>
+    <t>A-NZ PINT Invoice v1.0</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:peppol:pint:billing-1@aunz-1::2.1</t>
+  </si>
+  <si>
+    <t>A-NZ PINT Credit Note v1.0</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:peppol:pint:billing-1@aunz-1::2.1</t>
+  </si>
+  <si>
+    <t>A-NZ PINT Self-Billing Invoice v1.0</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:peppol:pint:selfbilling-1@aunz-1::2.1</t>
+  </si>
+  <si>
+    <t>A-NZ PINT Self-Billing Credit Note v1.0</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:peppol:pint:selfbilling-1@aunz-1::2.1</t>
+  </si>
+  <si>
+    <t>TICC-279</t>
   </si>
 </sst>
 </file>
@@ -2089,7 +2116,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2212,9 +2239,6 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2628,18 +2652,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
-  <dimension ref="A1:L229"/>
+  <dimension ref="A1:L237"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A207" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A227" sqref="A227"/>
+      <pane ySplit="1" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A237" sqref="A237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="47.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="103.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="97.28515625" style="5" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" style="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.140625" style="24" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="6" customWidth="1"/>
@@ -2928,7 +2952,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="37" customFormat="1" ht="30">
+    <row r="9" spans="1:12" s="37" customFormat="1" ht="45">
       <c r="A9" s="32" t="s">
         <v>28</v>
       </c>
@@ -3033,7 +3057,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="37" customFormat="1" ht="30">
+    <row r="12" spans="1:12" s="37" customFormat="1" ht="45">
       <c r="A12" s="32" t="s">
         <v>25</v>
       </c>
@@ -3101,7 +3125,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="37" customFormat="1" ht="30">
+    <row r="14" spans="1:12" s="37" customFormat="1" ht="45">
       <c r="A14" s="32" t="s">
         <v>101</v>
       </c>
@@ -3169,7 +3193,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="37" customFormat="1" ht="30">
+    <row r="16" spans="1:12" s="37" customFormat="1" ht="45">
       <c r="A16" s="32" t="s">
         <v>101</v>
       </c>
@@ -3271,7 +3295,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="37" customFormat="1" ht="30">
+    <row r="19" spans="1:12" s="37" customFormat="1" ht="45">
       <c r="A19" s="37" t="s">
         <v>96</v>
       </c>
@@ -3373,7 +3397,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="37" customFormat="1" ht="30">
+    <row r="22" spans="1:12" s="37" customFormat="1" ht="45">
       <c r="A22" s="37" t="s">
         <v>98</v>
       </c>
@@ -3441,7 +3465,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="37" customFormat="1" ht="30">
+    <row r="24" spans="1:12" s="37" customFormat="1" ht="45">
       <c r="A24" s="37" t="s">
         <v>98</v>
       </c>
@@ -4222,7 +4246,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" ht="30">
       <c r="A47" s="5" t="s">
         <v>61</v>
       </c>
@@ -4703,7 +4727,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="30">
+    <row r="63" spans="1:12" ht="45">
       <c r="A63" s="5" t="s">
         <v>479</v>
       </c>
@@ -5799,7 +5823,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="30">
+    <row r="96" spans="1:12" ht="45">
       <c r="A96" s="5" t="s">
         <v>202</v>
       </c>
@@ -6823,7 +6847,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="130" spans="1:12">
+    <row r="130" spans="1:12" ht="30">
       <c r="A130" s="5" t="s">
         <v>483</v>
       </c>
@@ -6887,7 +6911,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="132" spans="1:12">
+    <row r="132" spans="1:12" ht="30">
       <c r="A132" s="5" t="s">
         <v>485</v>
       </c>
@@ -7125,7 +7149,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="140" spans="1:12" ht="30">
+    <row r="140" spans="1:12" ht="45">
       <c r="A140" s="5" t="s">
         <v>313</v>
       </c>
@@ -7444,7 +7468,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="151" spans="1:12" ht="30">
+    <row r="151" spans="1:12" ht="45">
       <c r="A151" s="5" t="s">
         <v>359</v>
       </c>
@@ -7970,7 +7994,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="168" spans="1:12">
+    <row r="168" spans="1:12" ht="30">
       <c r="A168" s="5" t="s">
         <v>407</v>
       </c>
@@ -8066,7 +8090,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="171" spans="1:12">
+    <row r="171" spans="1:12" ht="30">
       <c r="A171" s="5" t="s">
         <v>412</v>
       </c>
@@ -8285,7 +8309,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="178" spans="1:12" ht="30">
+    <row r="178" spans="1:12" ht="45">
       <c r="A178" s="5" t="s">
         <v>437</v>
       </c>
@@ -8372,67 +8396,71 @@
         <v>130</v>
       </c>
     </row>
-    <row r="181" spans="1:12" ht="30">
-      <c r="A181" s="5" t="s">
+    <row r="181" spans="1:12" s="37" customFormat="1" ht="30">
+      <c r="A181" s="37" t="s">
         <v>487</v>
       </c>
-      <c r="B181" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C181" s="5" t="s">
+      <c r="B181" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="C181" s="37" t="s">
         <v>449</v>
       </c>
-      <c r="D181" s="29" t="s">
+      <c r="D181" s="38" t="s">
         <v>440</v>
       </c>
-      <c r="E181" s="24" t="s">
+      <c r="E181" s="34" t="s">
         <v>368</v>
       </c>
-      <c r="F181" s="44" t="s">
+      <c r="F181" s="41" t="s">
         <v>601</v>
       </c>
-      <c r="H181" s="5" t="s">
+      <c r="G181" s="36"/>
+      <c r="H181" s="37" t="s">
         <v>619</v>
       </c>
-      <c r="I181" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K181" s="24" t="s">
+      <c r="I181" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="J181" s="34"/>
+      <c r="K181" s="34" t="s">
         <v>451</v>
       </c>
-      <c r="L181" s="5" t="s">
+      <c r="L181" s="37" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="182" spans="1:12" ht="30">
-      <c r="A182" s="5" t="s">
+    <row r="182" spans="1:12" s="37" customFormat="1" ht="45">
+      <c r="A182" s="37" t="s">
         <v>488</v>
       </c>
-      <c r="B182" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C182" s="5" t="s">
+      <c r="B182" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="C182" s="37" t="s">
         <v>452</v>
       </c>
-      <c r="D182" s="29" t="s">
+      <c r="D182" s="38" t="s">
         <v>440</v>
       </c>
-      <c r="E182" s="24" t="s">
+      <c r="E182" s="34" t="s">
         <v>368</v>
       </c>
-      <c r="F182" s="44" t="s">
+      <c r="F182" s="41" t="s">
         <v>601</v>
       </c>
-      <c r="H182" s="5" t="s">
+      <c r="G182" s="36"/>
+      <c r="H182" s="37" t="s">
         <v>619</v>
       </c>
-      <c r="I182" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K182" s="24" t="s">
+      <c r="I182" s="37" t="b">
+        <v>1</v>
+      </c>
+      <c r="J182" s="34"/>
+      <c r="K182" s="34" t="s">
         <v>451</v>
       </c>
-      <c r="L182" s="5" t="s">
+      <c r="L182" s="37" t="s">
         <v>450</v>
       </c>
     </row>
@@ -8806,7 +8834,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="195" spans="1:12" ht="30">
+    <row r="195" spans="1:12" ht="45">
       <c r="A195" s="5" t="s">
         <v>526</v>
       </c>
@@ -9218,7 +9246,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="208" spans="1:12">
+    <row r="208" spans="1:12" ht="30">
       <c r="A208" s="5" t="s">
         <v>560</v>
       </c>
@@ -9250,7 +9278,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="209" spans="1:12">
+    <row r="209" spans="1:12" ht="30">
       <c r="A209" s="5" t="s">
         <v>565</v>
       </c>
@@ -9410,7 +9438,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="214" spans="1:12" ht="30">
+    <row r="214" spans="1:12" ht="45">
       <c r="A214" s="5" t="s">
         <v>588</v>
       </c>
@@ -9474,7 +9502,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="216" spans="1:12">
+    <row r="216" spans="1:12" ht="30">
       <c r="A216" s="5" t="s">
         <v>590</v>
       </c>
@@ -9660,7 +9688,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="222" spans="1:12" ht="30">
+    <row r="222" spans="1:12" ht="45">
       <c r="A222" s="5" t="s">
         <v>614</v>
       </c>
@@ -9837,7 +9865,7 @@
         <v>622</v>
       </c>
       <c r="I227" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J227" s="24">
         <v>3</v>
@@ -9849,7 +9877,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="228" spans="1:12">
+    <row r="228" spans="1:12" ht="30">
       <c r="A228" t="s">
         <v>629</v>
       </c>
@@ -9869,7 +9897,7 @@
         <v>622</v>
       </c>
       <c r="I228" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J228" s="24">
         <v>3</v>
@@ -9881,7 +9909,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="229" spans="1:12">
+    <row r="229" spans="1:12" ht="30">
       <c r="A229" t="s">
         <v>629</v>
       </c>
@@ -9901,7 +9929,7 @@
         <v>622</v>
       </c>
       <c r="I229" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J229" s="24">
         <v>3</v>
@@ -9913,8 +9941,264 @@
         <v>623</v>
       </c>
     </row>
+    <row r="230" spans="1:12">
+      <c r="A230" s="5" t="s">
+        <v>631</v>
+      </c>
+      <c r="B230" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C230" s="5" t="s">
+        <v>632</v>
+      </c>
+      <c r="D230" s="28" t="s">
+        <v>601</v>
+      </c>
+      <c r="E230" s="24" t="s">
+        <v>369</v>
+      </c>
+      <c r="H230" s="5" t="s">
+        <v>639</v>
+      </c>
+      <c r="I230" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J230" s="24">
+        <v>3</v>
+      </c>
+      <c r="K230" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="L230" s="5" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="231" spans="1:12" ht="30">
+      <c r="A231" s="5" t="s">
+        <v>633</v>
+      </c>
+      <c r="B231" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C231" s="5" t="s">
+        <v>634</v>
+      </c>
+      <c r="D231" s="28" t="s">
+        <v>601</v>
+      </c>
+      <c r="E231" s="24" t="s">
+        <v>369</v>
+      </c>
+      <c r="H231" s="5" t="s">
+        <v>639</v>
+      </c>
+      <c r="I231" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J231" s="24">
+        <v>3</v>
+      </c>
+      <c r="K231" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="L231" s="5" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="232" spans="1:12" ht="30">
+      <c r="A232" s="5" t="s">
+        <v>635</v>
+      </c>
+      <c r="B232" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C232" s="5" t="s">
+        <v>636</v>
+      </c>
+      <c r="D232" s="28" t="s">
+        <v>601</v>
+      </c>
+      <c r="E232" s="24" t="s">
+        <v>369</v>
+      </c>
+      <c r="H232" s="5" t="s">
+        <v>639</v>
+      </c>
+      <c r="I232" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J232" s="24">
+        <v>3</v>
+      </c>
+      <c r="K232" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="L232" s="5" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="233" spans="1:12" ht="30">
+      <c r="A233" s="5" t="s">
+        <v>637</v>
+      </c>
+      <c r="B233" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C233" s="5" t="s">
+        <v>638</v>
+      </c>
+      <c r="D233" s="28" t="s">
+        <v>601</v>
+      </c>
+      <c r="E233" s="24" t="s">
+        <v>369</v>
+      </c>
+      <c r="H233" s="5" t="s">
+        <v>639</v>
+      </c>
+      <c r="I233" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J233" s="24">
+        <v>3</v>
+      </c>
+      <c r="K233" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="L233" s="5" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="234" spans="1:12">
+      <c r="A234" s="5" t="s">
+        <v>631</v>
+      </c>
+      <c r="B234" s="5" t="s">
+        <v>620</v>
+      </c>
+      <c r="C234" s="5" t="s">
+        <v>632</v>
+      </c>
+      <c r="D234" s="28" t="s">
+        <v>601</v>
+      </c>
+      <c r="E234" s="24" t="s">
+        <v>369</v>
+      </c>
+      <c r="H234" s="5" t="s">
+        <v>639</v>
+      </c>
+      <c r="I234" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J234" s="24">
+        <v>3</v>
+      </c>
+      <c r="K234" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="L234" s="5" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="235" spans="1:12" ht="30">
+      <c r="A235" s="5" t="s">
+        <v>633</v>
+      </c>
+      <c r="B235" s="5" t="s">
+        <v>620</v>
+      </c>
+      <c r="C235" s="5" t="s">
+        <v>634</v>
+      </c>
+      <c r="D235" s="28" t="s">
+        <v>601</v>
+      </c>
+      <c r="E235" s="24" t="s">
+        <v>369</v>
+      </c>
+      <c r="H235" s="5" t="s">
+        <v>639</v>
+      </c>
+      <c r="I235" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J235" s="24">
+        <v>3</v>
+      </c>
+      <c r="K235" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="L235" s="5" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="236" spans="1:12" ht="30">
+      <c r="A236" s="5" t="s">
+        <v>635</v>
+      </c>
+      <c r="B236" s="5" t="s">
+        <v>620</v>
+      </c>
+      <c r="C236" s="5" t="s">
+        <v>636</v>
+      </c>
+      <c r="D236" s="28" t="s">
+        <v>601</v>
+      </c>
+      <c r="E236" s="24" t="s">
+        <v>369</v>
+      </c>
+      <c r="H236" s="5" t="s">
+        <v>639</v>
+      </c>
+      <c r="I236" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J236" s="24">
+        <v>3</v>
+      </c>
+      <c r="K236" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="L236" s="5" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="237" spans="1:12" ht="30">
+      <c r="A237" s="5" t="s">
+        <v>637</v>
+      </c>
+      <c r="B237" s="5" t="s">
+        <v>620</v>
+      </c>
+      <c r="C237" s="5" t="s">
+        <v>638</v>
+      </c>
+      <c r="D237" s="28" t="s">
+        <v>601</v>
+      </c>
+      <c r="E237" s="24" t="s">
+        <v>369</v>
+      </c>
+      <c r="H237" s="5" t="s">
+        <v>639</v>
+      </c>
+      <c r="I237" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J237" s="24">
+        <v>3</v>
+      </c>
+      <c r="K237" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="L237" s="5" t="s">
+        <v>539</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L229" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L237" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>